<commit_message>
upload before final reorg
</commit_message>
<xml_diff>
--- a/KZN_south_africa/param_files/calculated_param_gen/input_data/KZN_SA_model_parameters.xlsx
+++ b/KZN_south_africa/param_files/calculated_param_gen/input_data/KZN_SA_model_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/github/epi_model_HIV_TB/KZN_south_africa/param_files/calculated_param_gen/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A02EC10-D0AC-8140-A02A-7E6ED7132E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6737A6-66F3-F04D-8341-5BA8EC9A5327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="300" windowWidth="33340" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model_matched_parameters" sheetId="1" r:id="rId1"/>
@@ -939,7 +939,7 @@
       <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1184,15 +1184,15 @@
         <v>phi_3,</v>
       </c>
       <c r="I6" s="24">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
-        <v>0.67500000000000004</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="2"/>
-        <v>1.125</v>
+        <v>0.75</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>87</v>

</xml_diff>